<commit_message>
updated definitions after discussing with Hannah
</commit_message>
<xml_diff>
--- a/stats_country_ranks.xlsx
+++ b/stats_country_ranks.xlsx
@@ -35,12 +35,12 @@
     <t xml:space="preserve">New Zealand</t>
   </si>
   <si>
+    <t xml:space="preserve">Sierra Leone</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fiji</t>
   </si>
   <si>
-    <t xml:space="preserve">Sierra Leone</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cambodia</t>
   </si>
   <si>
@@ -59,6 +59,9 @@
     <t xml:space="preserve">Central African Republic</t>
   </si>
   <si>
+    <t xml:space="preserve">Lesotho</t>
+  </si>
+  <si>
     <t xml:space="preserve">Papua New Guinea</t>
   </si>
   <si>
@@ -71,39 +74,39 @@
     <t xml:space="preserve">Mongolia</t>
   </si>
   <si>
-    <t xml:space="preserve">Lesotho</t>
-  </si>
-  <si>
     <t xml:space="preserve">South Sudan</t>
   </si>
   <si>
+    <t xml:space="preserve">Bahamas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Botswana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liberia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burkina Faso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Congo</t>
+  </si>
+  <si>
     <t xml:space="preserve">Taiwan (Province of China)</t>
   </si>
   <si>
-    <t xml:space="preserve">Bahamas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Burkina Faso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Liberia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Congo</t>
+    <t xml:space="preserve">Belize</t>
   </si>
   <si>
     <t xml:space="preserve">Namibia</t>
   </si>
   <si>
-    <t xml:space="preserve">Botswana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Belize</t>
-  </si>
-  <si>
     <t xml:space="preserve">El Salvador</t>
   </si>
   <si>
+    <t xml:space="preserve">Guinea-Bissau</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mauritania</t>
   </si>
   <si>
@@ -113,7 +116,7 @@
     <t xml:space="preserve">Australia</t>
   </si>
   <si>
-    <t xml:space="preserve">Guinea-Bissau</t>
+    <t xml:space="preserve">Suriname</t>
   </si>
   <si>
     <t xml:space="preserve">Viet Nam</t>
@@ -122,70 +125,82 @@
     <t xml:space="preserve">Jordan</t>
   </si>
   <si>
+    <t xml:space="preserve">Sudan</t>
+  </si>
+  <si>
     <t xml:space="preserve">Iceland</t>
   </si>
   <si>
-    <t xml:space="preserve">Suriname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sudan</t>
+    <t xml:space="preserve">Malawi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Syrian Arab Republic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guyana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mali</t>
   </si>
   <si>
     <t xml:space="preserve">Andorra</t>
   </si>
   <si>
-    <t xml:space="preserve">Guyana</t>
+    <t xml:space="preserve">Madagascar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Myanmar</t>
   </si>
   <si>
     <t xml:space="preserve">Togo</t>
   </si>
   <si>
+    <t xml:space="preserve">Benin</t>
+  </si>
+  <si>
     <t xml:space="preserve">Palestine</t>
   </si>
   <si>
-    <t xml:space="preserve">Syrian Arab Republic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Benin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Madagascar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mali</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Malawi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Myanmar</t>
+    <t xml:space="preserve">Libya</t>
   </si>
   <si>
     <t xml:space="preserve">Angola</t>
   </si>
   <si>
+    <t xml:space="preserve">Cabo Verde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zimbabwe</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ghana</t>
   </si>
   <si>
-    <t xml:space="preserve">Cabo Verde</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zimbabwe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Libya</t>
+    <t xml:space="preserve">Montenegro</t>
   </si>
   <si>
     <t xml:space="preserve">Somalia</t>
   </si>
   <si>
-    <t xml:space="preserve">Montenegro</t>
+    <t xml:space="preserve">Eswatini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gabon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mozambique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zambia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guinea</t>
   </si>
   <si>
     <t xml:space="preserve">Côte d'Ivoire</t>
   </si>
   <si>
-    <t xml:space="preserve">Gabon</t>
+    <t xml:space="preserve">Jamaica</t>
   </si>
   <si>
     <t xml:space="preserve">Nigeria</t>
@@ -194,10 +209,10 @@
     <t xml:space="preserve">Cameroon</t>
   </si>
   <si>
-    <t xml:space="preserve">Guinea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jamaica</t>
+    <t xml:space="preserve">Rwanda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haiti</t>
   </si>
   <si>
     <t xml:space="preserve">Nepal</t>
@@ -212,63 +227,57 @@
     <t xml:space="preserve">Oman</t>
   </si>
   <si>
-    <t xml:space="preserve">Zambia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rwanda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mozambique</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tunisia</t>
   </si>
   <si>
+    <t xml:space="preserve">Kyrgyzstan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Venezuela (Bolivarian Republic of)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Estonia</t>
   </si>
   <si>
-    <t xml:space="preserve">Eswatini</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Haiti</t>
-  </si>
-  <si>
     <t xml:space="preserve">Maldives</t>
   </si>
   <si>
     <t xml:space="preserve">Afghanistan</t>
   </si>
   <si>
+    <t xml:space="preserve">Sri Lanka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Türkiye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Albania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ethiopia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hungary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kazakhstan</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hong Kong Special Administrative Region of China</t>
   </si>
   <si>
-    <t xml:space="preserve">Venezuela (Bolivarian Republic of)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sri Lanka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hungary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kyrgyzstan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Albania</t>
-  </si>
-  <si>
     <t xml:space="preserve">Latvia</t>
   </si>
   <si>
     <t xml:space="preserve">Ecuador</t>
   </si>
   <si>
+    <t xml:space="preserve">Kenya</t>
+  </si>
+  <si>
     <t xml:space="preserve">Senegal</t>
   </si>
   <si>
-    <t xml:space="preserve">Türkiye</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dominican Republic</t>
   </si>
   <si>
@@ -278,51 +287,45 @@
     <t xml:space="preserve">Slovenia</t>
   </si>
   <si>
+    <t xml:space="preserve">Uruguay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lithuania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Malaysia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paraguay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panama</t>
+  </si>
+  <si>
     <t xml:space="preserve">Thailand</t>
   </si>
   <si>
-    <t xml:space="preserve">Ethiopia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kazakhstan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lithuania</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Malaysia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paraguay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kenya</t>
+    <t xml:space="preserve">Honduras</t>
   </si>
   <si>
     <t xml:space="preserve">Ukraine</t>
   </si>
   <si>
-    <t xml:space="preserve">Panama</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bangladesh</t>
   </si>
   <si>
+    <t xml:space="preserve">Bolivia (Plurinational State of)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Costa Rica</t>
   </si>
   <si>
     <t xml:space="preserve">Croatia</t>
   </si>
   <si>
-    <t xml:space="preserve">Cuba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uruguay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Honduras</t>
-  </si>
-  <si>
     <t xml:space="preserve">Republic of Moldova</t>
   </si>
   <si>
@@ -332,7 +335,13 @@
     <t xml:space="preserve">Colombia</t>
   </si>
   <si>
-    <t xml:space="preserve">Bolivia (Plurinational State of)</t>
+    <t xml:space="preserve">Guatemala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uzbekistan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Democratic Republic of the Congo</t>
   </si>
   <si>
     <t xml:space="preserve">Algeria</t>
@@ -341,9 +350,6 @@
     <t xml:space="preserve">Argentina</t>
   </si>
   <si>
-    <t xml:space="preserve">Democratic Republic of the Congo</t>
-  </si>
-  <si>
     <t xml:space="preserve">Egypt</t>
   </si>
   <si>
@@ -368,27 +374,21 @@
     <t xml:space="preserve">South Africa</t>
   </si>
   <si>
+    <t xml:space="preserve">Chile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mexico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Morocco</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sweden</t>
   </si>
   <si>
     <t xml:space="preserve">United Arab Emirates</t>
   </si>
   <si>
-    <t xml:space="preserve">Chile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guatemala</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mexico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Morocco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uzbekistan</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bosnia and Herzegovina</t>
   </si>
   <si>
@@ -401,36 +401,39 @@
     <t xml:space="preserve">Serbia</t>
   </si>
   <si>
+    <t xml:space="preserve">Indonesia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pakistan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qatar</t>
+  </si>
+  <si>
     <t xml:space="preserve">Belgium</t>
   </si>
   <si>
-    <t xml:space="preserve">Indonesia</t>
-  </si>
-  <si>
     <t xml:space="preserve">Lebanon</t>
   </si>
   <si>
+    <t xml:space="preserve">Poland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Russian Federation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brazil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">India</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luxembourg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Philippines</t>
   </si>
   <si>
-    <t xml:space="preserve">Poland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Russian Federation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brazil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">India</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Luxembourg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pakistan</t>
-  </si>
-  <si>
     <t xml:space="preserve">Romania</t>
   </si>
   <si>
@@ -464,15 +467,12 @@
     <t xml:space="preserve">Italy</t>
   </si>
   <si>
+    <t xml:space="preserve">Austria</t>
+  </si>
+  <si>
     <t xml:space="preserve">United Kingdom</t>
   </si>
   <si>
-    <t xml:space="preserve">Qatar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Austria</t>
-  </si>
-  <si>
     <t xml:space="preserve">Germany</t>
   </si>
   <si>
@@ -488,16 +488,16 @@
     <t xml:space="preserve">Singapore</t>
   </si>
   <si>
+    <t xml:space="preserve">Japan</t>
+  </si>
+  <si>
     <t xml:space="preserve">Republic of Korea</t>
   </si>
   <si>
-    <t xml:space="preserve">Japan</t>
+    <t xml:space="preserve">United States of America</t>
   </si>
   <si>
     <t xml:space="preserve">China</t>
-  </si>
-  <si>
-    <t xml:space="preserve">United States of America</t>
   </si>
 </sst>
 </file>
@@ -854,10 +854,10 @@
         <v>110</v>
       </c>
       <c r="C2" t="n">
-        <v>927</v>
+        <v>932</v>
       </c>
       <c r="D2" t="n">
-        <v>927</v>
+        <v>932</v>
       </c>
       <c r="E2" t="n">
         <v>157</v>
@@ -868,13 +868,13 @@
         <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="C3" t="n">
         <v>455</v>
       </c>
       <c r="D3" t="n">
-        <v>457</v>
+        <v>463</v>
       </c>
       <c r="E3" t="n">
         <v>156</v>
@@ -885,13 +885,13 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>140</v>
+        <v>166</v>
       </c>
       <c r="C4" t="n">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="D4" t="n">
-        <v>398</v>
+        <v>420</v>
       </c>
       <c r="E4" t="n">
         <v>155</v>
@@ -902,13 +902,13 @@
         <v>8</v>
       </c>
       <c r="B5" t="n">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="C5" t="n">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="D5" t="n">
-        <v>391</v>
+        <v>415</v>
       </c>
       <c r="E5" t="n">
         <v>154</v>
@@ -922,10 +922,10 @@
         <v>110</v>
       </c>
       <c r="C6" t="n">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="D6" t="n">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="E6" t="n">
         <v>153</v>
@@ -936,13 +936,13 @@
         <v>10</v>
       </c>
       <c r="B7" t="n">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C7" t="n">
         <v>247</v>
       </c>
       <c r="D7" t="n">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="E7" t="n">
         <v>152</v>
@@ -953,13 +953,13 @@
         <v>11</v>
       </c>
       <c r="B8" t="n">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="C8" t="n">
         <v>247</v>
       </c>
       <c r="D8" t="n">
-        <v>274</v>
+        <v>291</v>
       </c>
       <c r="E8" t="n">
         <v>151</v>
@@ -970,13 +970,13 @@
         <v>12</v>
       </c>
       <c r="B9" t="n">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="C9" t="n">
         <v>216</v>
       </c>
       <c r="D9" t="n">
-        <v>263</v>
+        <v>278</v>
       </c>
       <c r="E9" t="n">
         <v>150</v>
@@ -987,13 +987,13 @@
         <v>13</v>
       </c>
       <c r="B10" t="n">
-        <v>137</v>
+        <v>155</v>
       </c>
       <c r="C10" t="n">
         <v>223</v>
       </c>
       <c r="D10" t="n">
-        <v>250</v>
+        <v>268</v>
       </c>
       <c r="E10" t="n">
         <v>149</v>
@@ -1004,13 +1004,13 @@
         <v>14</v>
       </c>
       <c r="B11" t="n">
-        <v>141</v>
+        <v>170</v>
       </c>
       <c r="C11" t="n">
         <v>207</v>
       </c>
       <c r="D11" t="n">
-        <v>238</v>
+        <v>267</v>
       </c>
       <c r="E11" t="n">
         <v>148</v>
@@ -1021,13 +1021,13 @@
         <v>15</v>
       </c>
       <c r="B12" t="n">
-        <v>137</v>
+        <v>296</v>
       </c>
       <c r="C12" t="n">
-        <v>202</v>
+        <v>75</v>
       </c>
       <c r="D12" t="n">
-        <v>229</v>
+        <v>261</v>
       </c>
       <c r="E12" t="n">
         <v>147</v>
@@ -1038,13 +1038,13 @@
         <v>16</v>
       </c>
       <c r="B13" t="n">
-        <v>137</v>
+        <v>155</v>
       </c>
       <c r="C13" t="n">
-        <v>177</v>
+        <v>202</v>
       </c>
       <c r="D13" t="n">
-        <v>204</v>
+        <v>247</v>
       </c>
       <c r="E13" t="n">
         <v>146</v>
@@ -1055,13 +1055,13 @@
         <v>17</v>
       </c>
       <c r="B14" t="n">
-        <v>293</v>
+        <v>150</v>
       </c>
       <c r="C14" t="n">
-        <v>20</v>
+        <v>177</v>
       </c>
       <c r="D14" t="n">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="E14" t="n">
         <v>145</v>
@@ -1072,13 +1072,13 @@
         <v>18</v>
       </c>
       <c r="B15" t="n">
-        <v>137</v>
+        <v>299</v>
       </c>
       <c r="C15" t="n">
-        <v>169</v>
+        <v>20</v>
       </c>
       <c r="D15" t="n">
-        <v>196</v>
+        <v>209</v>
       </c>
       <c r="E15" t="n">
         <v>144</v>
@@ -1089,13 +1089,13 @@
         <v>19</v>
       </c>
       <c r="B16" t="n">
-        <v>224</v>
+        <v>145</v>
       </c>
       <c r="C16" t="n">
-        <v>75</v>
+        <v>169</v>
       </c>
       <c r="D16" t="n">
-        <v>189</v>
+        <v>204</v>
       </c>
       <c r="E16" t="n">
         <v>143</v>
@@ -1106,13 +1106,13 @@
         <v>20</v>
       </c>
       <c r="B17" t="n">
-        <v>137</v>
+        <v>171</v>
       </c>
       <c r="C17" t="n">
         <v>143</v>
       </c>
       <c r="D17" t="n">
-        <v>170</v>
+        <v>204</v>
       </c>
       <c r="E17" t="n">
         <v>142</v>
@@ -1123,13 +1123,13 @@
         <v>21</v>
       </c>
       <c r="B18" t="n">
-        <v>110</v>
+        <v>161</v>
       </c>
       <c r="C18" t="n">
-        <v>167</v>
+        <v>128</v>
       </c>
       <c r="D18" t="n">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="E18" t="n">
         <v>141</v>
@@ -1140,13 +1140,13 @@
         <v>22</v>
       </c>
       <c r="B19" t="n">
-        <v>147</v>
+        <v>165</v>
       </c>
       <c r="C19" t="n">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="D19" t="n">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="E19" t="n">
         <v>140</v>
@@ -1157,13 +1157,13 @@
         <v>23</v>
       </c>
       <c r="B20" t="n">
-        <v>213</v>
+        <v>151</v>
       </c>
       <c r="C20" t="n">
-        <v>59</v>
+        <v>131</v>
       </c>
       <c r="D20" t="n">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="E20" t="n">
         <v>139</v>
@@ -1174,13 +1174,13 @@
         <v>24</v>
       </c>
       <c r="B21" t="n">
-        <v>137</v>
+        <v>221</v>
       </c>
       <c r="C21" t="n">
-        <v>131</v>
+        <v>59</v>
       </c>
       <c r="D21" t="n">
-        <v>158</v>
+        <v>170</v>
       </c>
       <c r="E21" t="n">
         <v>138</v>
@@ -1191,13 +1191,13 @@
         <v>25</v>
       </c>
       <c r="B22" t="n">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="C22" t="n">
         <v>103</v>
       </c>
       <c r="D22" t="n">
-        <v>157</v>
+        <v>170</v>
       </c>
       <c r="E22" t="n">
         <v>137</v>
@@ -1208,13 +1208,13 @@
         <v>26</v>
       </c>
       <c r="B23" t="n">
-        <v>178</v>
+        <v>110</v>
       </c>
       <c r="C23" t="n">
-        <v>78</v>
+        <v>169</v>
       </c>
       <c r="D23" t="n">
-        <v>146</v>
+        <v>169</v>
       </c>
       <c r="E23" t="n">
         <v>136</v>
@@ -1225,13 +1225,13 @@
         <v>27</v>
       </c>
       <c r="B24" t="n">
-        <v>137</v>
+        <v>158</v>
       </c>
       <c r="C24" t="n">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D24" t="n">
-        <v>145</v>
+        <v>161</v>
       </c>
       <c r="E24" t="n">
         <v>135</v>
@@ -1242,13 +1242,13 @@
         <v>28</v>
       </c>
       <c r="B25" t="n">
-        <v>137</v>
+        <v>190</v>
       </c>
       <c r="C25" t="n">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="D25" t="n">
-        <v>140</v>
+        <v>158</v>
       </c>
       <c r="E25" t="n">
         <v>134</v>
@@ -1259,16 +1259,16 @@
         <v>29</v>
       </c>
       <c r="B26" t="n">
-        <v>242</v>
+        <v>259</v>
       </c>
       <c r="C26" t="n">
         <v>6</v>
       </c>
       <c r="D26" t="n">
-        <v>138</v>
+        <v>155</v>
       </c>
       <c r="E26" t="n">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="27">
@@ -1276,16 +1276,16 @@
         <v>30</v>
       </c>
       <c r="B27" t="n">
-        <v>137</v>
+        <v>187</v>
       </c>
       <c r="C27" t="n">
-        <v>111</v>
+        <v>74</v>
       </c>
       <c r="D27" t="n">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="E27" t="n">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28">
@@ -1293,13 +1293,13 @@
         <v>31</v>
       </c>
       <c r="B28" t="n">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="C28" t="n">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="D28" t="n">
-        <v>135</v>
+        <v>150</v>
       </c>
       <c r="E28" t="n">
         <v>131</v>
@@ -1310,13 +1310,13 @@
         <v>32</v>
       </c>
       <c r="B29" t="n">
-        <v>125</v>
+        <v>155</v>
       </c>
       <c r="C29" t="n">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="D29" t="n">
-        <v>128</v>
+        <v>147</v>
       </c>
       <c r="E29" t="n">
         <v>130</v>
@@ -1327,13 +1327,13 @@
         <v>33</v>
       </c>
       <c r="B30" t="n">
-        <v>164</v>
+        <v>131</v>
       </c>
       <c r="C30" t="n">
-        <v>74</v>
+        <v>113</v>
       </c>
       <c r="D30" t="n">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="E30" t="n">
         <v>129</v>
@@ -1344,16 +1344,16 @@
         <v>34</v>
       </c>
       <c r="B31" t="n">
-        <v>110</v>
+        <v>161</v>
       </c>
       <c r="C31" t="n">
-        <v>119</v>
+        <v>72</v>
       </c>
       <c r="D31" t="n">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="E31" t="n">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32">
@@ -1361,16 +1361,16 @@
         <v>35</v>
       </c>
       <c r="B32" t="n">
-        <v>210</v>
+        <v>110</v>
       </c>
       <c r="C32" t="n">
-        <v>16</v>
+        <v>123</v>
       </c>
       <c r="D32" t="n">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="E32" t="n">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33">
@@ -1378,13 +1378,13 @@
         <v>36</v>
       </c>
       <c r="B33" t="n">
-        <v>142</v>
+        <v>216</v>
       </c>
       <c r="C33" t="n">
-        <v>80</v>
+        <v>16</v>
       </c>
       <c r="D33" t="n">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="E33" t="n">
         <v>126</v>
@@ -1395,13 +1395,13 @@
         <v>37</v>
       </c>
       <c r="B34" t="n">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C34" t="n">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="D34" t="n">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="E34" t="n">
         <v>125</v>
@@ -1412,13 +1412,13 @@
         <v>38</v>
       </c>
       <c r="B35" t="n">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="C35" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D35" t="n">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="E35" t="n">
         <v>124</v>
@@ -1429,13 +1429,13 @@
         <v>39</v>
       </c>
       <c r="B36" t="n">
-        <v>136</v>
+        <v>173</v>
       </c>
       <c r="C36" t="n">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="D36" t="n">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="E36" t="n">
         <v>123</v>
@@ -1446,13 +1446,13 @@
         <v>40</v>
       </c>
       <c r="B37" t="n">
-        <v>137</v>
+        <v>158</v>
       </c>
       <c r="C37" t="n">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="D37" t="n">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="E37" t="n">
         <v>122</v>
@@ -1463,13 +1463,13 @@
         <v>41</v>
       </c>
       <c r="B38" t="n">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="C38" t="n">
         <v>74</v>
       </c>
       <c r="D38" t="n">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="E38" t="n">
         <v>121</v>
@@ -1480,13 +1480,13 @@
         <v>42</v>
       </c>
       <c r="B39" t="n">
-        <v>181</v>
+        <v>160</v>
       </c>
       <c r="C39" t="n">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="D39" t="n">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="E39" t="n">
         <v>120</v>
@@ -1497,13 +1497,13 @@
         <v>43</v>
       </c>
       <c r="B40" t="n">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C40" t="n">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="D40" t="n">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="E40" t="n">
         <v>119</v>
@@ -1514,13 +1514,13 @@
         <v>44</v>
       </c>
       <c r="B41" t="n">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="C41" t="n">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="D41" t="n">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="E41" t="n">
         <v>118</v>
@@ -1531,13 +1531,13 @@
         <v>45</v>
       </c>
       <c r="B42" t="n">
-        <v>138</v>
+        <v>162</v>
       </c>
       <c r="C42" t="n">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D42" t="n">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="E42" t="n">
         <v>117</v>
@@ -1548,13 +1548,13 @@
         <v>46</v>
       </c>
       <c r="B43" t="n">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="C43" t="n">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="D43" t="n">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="E43" t="n">
         <v>116</v>
@@ -1565,13 +1565,13 @@
         <v>47</v>
       </c>
       <c r="B44" t="n">
-        <v>142</v>
+        <v>164</v>
       </c>
       <c r="C44" t="n">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D44" t="n">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="E44" t="n">
         <v>115</v>
@@ -1582,13 +1582,13 @@
         <v>48</v>
       </c>
       <c r="B45" t="n">
-        <v>137</v>
+        <v>187</v>
       </c>
       <c r="C45" t="n">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="D45" t="n">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="E45" t="n">
         <v>114</v>
@@ -1599,13 +1599,13 @@
         <v>49</v>
       </c>
       <c r="B46" t="n">
-        <v>144</v>
+        <v>166</v>
       </c>
       <c r="C46" t="n">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D46" t="n">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="E46" t="n">
         <v>113</v>
@@ -1616,13 +1616,13 @@
         <v>50</v>
       </c>
       <c r="B47" t="n">
-        <v>137</v>
+        <v>162</v>
       </c>
       <c r="C47" t="n">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D47" t="n">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="E47" t="n">
         <v>112</v>
@@ -1633,13 +1633,13 @@
         <v>51</v>
       </c>
       <c r="B48" t="n">
-        <v>137</v>
+        <v>155</v>
       </c>
       <c r="C48" t="n">
         <v>51</v>
       </c>
       <c r="D48" t="n">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="E48" t="n">
         <v>111</v>
@@ -1650,13 +1650,13 @@
         <v>52</v>
       </c>
       <c r="B49" t="n">
-        <v>144</v>
+        <v>162</v>
       </c>
       <c r="C49" t="n">
         <v>44</v>
       </c>
       <c r="D49" t="n">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="E49" t="n">
         <v>110</v>
@@ -1667,13 +1667,13 @@
         <v>53</v>
       </c>
       <c r="B50" t="n">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C50" t="n">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="D50" t="n">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="E50" t="n">
         <v>109</v>
@@ -1684,13 +1684,13 @@
         <v>54</v>
       </c>
       <c r="B51" t="n">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="C51" t="n">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D51" t="n">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="E51" t="n">
         <v>108</v>
@@ -1701,13 +1701,13 @@
         <v>55</v>
       </c>
       <c r="B52" t="n">
-        <v>137</v>
+        <v>155</v>
       </c>
       <c r="C52" t="n">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D52" t="n">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="E52" t="n">
         <v>107</v>
@@ -1718,16 +1718,16 @@
         <v>56</v>
       </c>
       <c r="B53" t="n">
-        <v>110</v>
+        <v>157</v>
       </c>
       <c r="C53" t="n">
-        <v>71</v>
+        <v>36</v>
       </c>
       <c r="D53" t="n">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="E53" t="n">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="54">
@@ -1735,16 +1735,16 @@
         <v>57</v>
       </c>
       <c r="B54" t="n">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="C54" t="n">
         <v>44</v>
       </c>
       <c r="D54" t="n">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="E54" t="n">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="55">
@@ -1752,13 +1752,13 @@
         <v>58</v>
       </c>
       <c r="B55" t="n">
-        <v>128</v>
+        <v>157</v>
       </c>
       <c r="C55" t="n">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="D55" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="E55" t="n">
         <v>104</v>
@@ -1769,13 +1769,13 @@
         <v>59</v>
       </c>
       <c r="B56" t="n">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="C56" t="n">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="D56" t="n">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="E56" t="n">
         <v>103</v>
@@ -1786,16 +1786,16 @@
         <v>60</v>
       </c>
       <c r="B57" t="n">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="C57" t="n">
         <v>13</v>
       </c>
       <c r="D57" t="n">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="E57" t="n">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="58">
@@ -1803,16 +1803,16 @@
         <v>61</v>
       </c>
       <c r="B58" t="n">
-        <v>149</v>
+        <v>110</v>
       </c>
       <c r="C58" t="n">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="D58" t="n">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="E58" t="n">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="59">
@@ -1820,16 +1820,16 @@
         <v>62</v>
       </c>
       <c r="B59" t="n">
-        <v>110</v>
+        <v>158</v>
       </c>
       <c r="C59" t="n">
-        <v>67</v>
+        <v>28</v>
       </c>
       <c r="D59" t="n">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="E59" t="n">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="60">
@@ -1837,16 +1837,16 @@
         <v>63</v>
       </c>
       <c r="B60" t="n">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C60" t="n">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="D60" t="n">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="E60" t="n">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="61">
@@ -1854,13 +1854,13 @@
         <v>64</v>
       </c>
       <c r="B61" t="n">
-        <v>140</v>
+        <v>176</v>
       </c>
       <c r="C61" t="n">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D61" t="n">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="E61" t="n">
         <v>98</v>
@@ -1871,16 +1871,16 @@
         <v>65</v>
       </c>
       <c r="B62" t="n">
-        <v>138</v>
+        <v>155</v>
       </c>
       <c r="C62" t="n">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D62" t="n">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="E62" t="n">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="63">
@@ -1888,16 +1888,16 @@
         <v>66</v>
       </c>
       <c r="B63" t="n">
-        <v>137</v>
+        <v>158</v>
       </c>
       <c r="C63" t="n">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D63" t="n">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="E63" t="n">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="64">
@@ -1905,13 +1905,13 @@
         <v>67</v>
       </c>
       <c r="B64" t="n">
-        <v>143</v>
+        <v>110</v>
       </c>
       <c r="C64" t="n">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="D64" t="n">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="E64" t="n">
         <v>95</v>
@@ -1922,13 +1922,13 @@
         <v>68</v>
       </c>
       <c r="B65" t="n">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C65" t="n">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D65" t="n">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="E65" t="n">
         <v>94</v>
@@ -1939,13 +1939,13 @@
         <v>69</v>
       </c>
       <c r="B66" t="n">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="C66" t="n">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D66" t="n">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="E66" t="n">
         <v>93</v>
@@ -1956,16 +1956,16 @@
         <v>70</v>
       </c>
       <c r="B67" t="n">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="C67" t="n">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D67" t="n">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="E67" t="n">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="68">
@@ -1973,16 +1973,16 @@
         <v>71</v>
       </c>
       <c r="B68" t="n">
-        <v>129</v>
+        <v>145</v>
       </c>
       <c r="C68" t="n">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D68" t="n">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="E68" t="n">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="69">
@@ -1990,13 +1990,13 @@
         <v>72</v>
       </c>
       <c r="B69" t="n">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="C69" t="n">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D69" t="n">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="E69" t="n">
         <v>90</v>
@@ -2007,13 +2007,13 @@
         <v>73</v>
       </c>
       <c r="B70" t="n">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="C70" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D70" t="n">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="E70" t="n">
         <v>89</v>
@@ -2024,13 +2024,13 @@
         <v>74</v>
       </c>
       <c r="B71" t="n">
-        <v>124</v>
+        <v>146</v>
       </c>
       <c r="C71" t="n">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="D71" t="n">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="E71" t="n">
         <v>88</v>
@@ -2041,13 +2041,13 @@
         <v>75</v>
       </c>
       <c r="B72" t="n">
-        <v>110</v>
+        <v>141</v>
       </c>
       <c r="C72" t="n">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="D72" t="n">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="E72" t="n">
         <v>87</v>
@@ -2058,13 +2058,13 @@
         <v>76</v>
       </c>
       <c r="B73" t="n">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C73" t="n">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="D73" t="n">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="E73" t="n">
         <v>86</v>
@@ -2078,10 +2078,10 @@
         <v>110</v>
       </c>
       <c r="C74" t="n">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D74" t="n">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="E74" t="n">
         <v>85</v>
@@ -2092,13 +2092,13 @@
         <v>78</v>
       </c>
       <c r="B75" t="n">
-        <v>138</v>
+        <v>161</v>
       </c>
       <c r="C75" t="n">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D75" t="n">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="E75" t="n">
         <v>84</v>
@@ -2109,16 +2109,16 @@
         <v>79</v>
       </c>
       <c r="B76" t="n">
-        <v>137</v>
+        <v>156</v>
       </c>
       <c r="C76" t="n">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="D76" t="n">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="E76" t="n">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="77">
@@ -2126,13 +2126,13 @@
         <v>80</v>
       </c>
       <c r="B77" t="n">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C77" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D77" t="n">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="E77" t="n">
         <v>82</v>
@@ -2143,13 +2143,13 @@
         <v>81</v>
       </c>
       <c r="B78" t="n">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="C78" t="n">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D78" t="n">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="E78" t="n">
         <v>81</v>
@@ -2160,16 +2160,16 @@
         <v>82</v>
       </c>
       <c r="B79" t="n">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="C79" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D79" t="n">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="E79" t="n">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="80">
@@ -2177,16 +2177,16 @@
         <v>83</v>
       </c>
       <c r="B80" t="n">
-        <v>137</v>
+        <v>110</v>
       </c>
       <c r="C80" t="n">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="D80" t="n">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="E80" t="n">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="81">
@@ -2194,13 +2194,13 @@
         <v>84</v>
       </c>
       <c r="B81" t="n">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="C81" t="n">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="D81" t="n">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="E81" t="n">
         <v>78</v>
@@ -2211,16 +2211,16 @@
         <v>85</v>
       </c>
       <c r="B82" t="n">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C82" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D82" t="n">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E82" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="83">
@@ -2228,16 +2228,16 @@
         <v>86</v>
       </c>
       <c r="B83" t="n">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="C83" t="n">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="D83" t="n">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E83" t="n">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="84">
@@ -2245,16 +2245,16 @@
         <v>87</v>
       </c>
       <c r="B84" t="n">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="C84" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D84" t="n">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E84" t="n">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="85">
@@ -2262,16 +2262,16 @@
         <v>88</v>
       </c>
       <c r="B85" t="n">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="C85" t="n">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="D85" t="n">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="E85" t="n">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="86">
@@ -2279,16 +2279,16 @@
         <v>89</v>
       </c>
       <c r="B86" t="n">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C86" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D86" t="n">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E86" t="n">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="87">
@@ -2296,16 +2296,16 @@
         <v>90</v>
       </c>
       <c r="B87" t="n">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C87" t="n">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D87" t="n">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E87" t="n">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="88">
@@ -2313,16 +2313,16 @@
         <v>91</v>
       </c>
       <c r="B88" t="n">
-        <v>128</v>
+        <v>149</v>
       </c>
       <c r="C88" t="n">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D88" t="n">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E88" t="n">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="89">
@@ -2330,16 +2330,16 @@
         <v>92</v>
       </c>
       <c r="B89" t="n">
-        <v>110</v>
+        <v>147</v>
       </c>
       <c r="C89" t="n">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="D89" t="n">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="E89" t="n">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="90">
@@ -2347,16 +2347,16 @@
         <v>93</v>
       </c>
       <c r="B90" t="n">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C90" t="n">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="D90" t="n">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="E90" t="n">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="91">
@@ -2364,16 +2364,16 @@
         <v>94</v>
       </c>
       <c r="B91" t="n">
-        <v>137</v>
+        <v>110</v>
       </c>
       <c r="C91" t="n">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="D91" t="n">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E91" t="n">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="92">
@@ -2381,13 +2381,13 @@
         <v>95</v>
       </c>
       <c r="B92" t="n">
-        <v>114</v>
+        <v>148</v>
       </c>
       <c r="C92" t="n">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="D92" t="n">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E92" t="n">
         <v>68</v>
@@ -2398,16 +2398,16 @@
         <v>96</v>
       </c>
       <c r="B93" t="n">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="C93" t="n">
         <v>4</v>
       </c>
       <c r="D93" t="n">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E93" t="n">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="94">
@@ -2415,16 +2415,16 @@
         <v>97</v>
       </c>
       <c r="B94" t="n">
-        <v>137</v>
+        <v>111</v>
       </c>
       <c r="C94" t="n">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="D94" t="n">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="E94" t="n">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="95">
@@ -2432,16 +2432,16 @@
         <v>98</v>
       </c>
       <c r="B95" t="n">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C95" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D95" t="n">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E95" t="n">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="96">
@@ -2449,16 +2449,16 @@
         <v>99</v>
       </c>
       <c r="B96" t="n">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="C96" t="n">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="D96" t="n">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E96" t="n">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="97">
@@ -2466,16 +2466,16 @@
         <v>100</v>
       </c>
       <c r="B97" t="n">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="C97" t="n">
         <v>10</v>
       </c>
       <c r="D97" t="n">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E97" t="n">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="98">
@@ -2483,16 +2483,16 @@
         <v>101</v>
       </c>
       <c r="B98" t="n">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="C98" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D98" t="n">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E98" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="99">
@@ -2500,16 +2500,16 @@
         <v>102</v>
       </c>
       <c r="B99" t="n">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="C99" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D99" t="n">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="E99" t="n">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="100">
@@ -2517,16 +2517,16 @@
         <v>103</v>
       </c>
       <c r="B100" t="n">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="C100" t="n">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="D100" t="n">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="E100" t="n">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="101">
@@ -2534,16 +2534,16 @@
         <v>104</v>
       </c>
       <c r="B101" t="n">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="C101" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D101" t="n">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E101" t="n">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="102">
@@ -2551,16 +2551,16 @@
         <v>105</v>
       </c>
       <c r="B102" t="n">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C102" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D102" t="n">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="E102" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="103">
@@ -2568,16 +2568,16 @@
         <v>106</v>
       </c>
       <c r="B103" t="n">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="C103" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D103" t="n">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="E103" t="n">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="104">
@@ -2585,16 +2585,16 @@
         <v>107</v>
       </c>
       <c r="B104" t="n">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="C104" t="n">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D104" t="n">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E104" t="n">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="105">
@@ -2602,13 +2602,13 @@
         <v>108</v>
       </c>
       <c r="B105" t="n">
-        <v>134</v>
+        <v>150</v>
       </c>
       <c r="C105" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D105" t="n">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E105" t="n">
         <v>55</v>
@@ -2619,13 +2619,13 @@
         <v>109</v>
       </c>
       <c r="B106" t="n">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="C106" t="n">
         <v>4</v>
       </c>
       <c r="D106" t="n">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="E106" t="n">
         <v>53</v>
@@ -2636,13 +2636,13 @@
         <v>110</v>
       </c>
       <c r="B107" t="n">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="C107" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D107" t="n">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="E107" t="n">
         <v>52</v>
@@ -2653,16 +2653,16 @@
         <v>111</v>
       </c>
       <c r="B108" t="n">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C108" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D108" t="n">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="E108" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="109">
@@ -2670,16 +2670,16 @@
         <v>112</v>
       </c>
       <c r="B109" t="n">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="C109" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="D109" t="n">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="E109" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="110">
@@ -2687,16 +2687,16 @@
         <v>113</v>
       </c>
       <c r="B110" t="n">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C110" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D110" t="n">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E110" t="n">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="111">
@@ -2704,13 +2704,13 @@
         <v>114</v>
       </c>
       <c r="B111" t="n">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="C111" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D111" t="n">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E111" t="n">
         <v>48</v>
@@ -2721,13 +2721,13 @@
         <v>115</v>
       </c>
       <c r="B112" t="n">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C112" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D112" t="n">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E112" t="n">
         <v>49</v>
@@ -2738,16 +2738,16 @@
         <v>116</v>
       </c>
       <c r="B113" t="n">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="C113" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D113" t="n">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E113" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="114">
@@ -2755,16 +2755,16 @@
         <v>117</v>
       </c>
       <c r="B114" t="n">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="C114" t="n">
         <v>4</v>
       </c>
       <c r="D114" t="n">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E114" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="115">
@@ -2772,16 +2772,16 @@
         <v>118</v>
       </c>
       <c r="B115" t="n">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="C115" t="n">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D115" t="n">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E115" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="116">
@@ -2789,16 +2789,16 @@
         <v>119</v>
       </c>
       <c r="B116" t="n">
-        <v>110</v>
+        <v>141</v>
       </c>
       <c r="C116" t="n">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="D116" t="n">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E116" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="117">
@@ -2806,13 +2806,13 @@
         <v>120</v>
       </c>
       <c r="B117" t="n">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="C117" t="n">
         <v>6</v>
       </c>
       <c r="D117" t="n">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E117" t="n">
         <v>42</v>
@@ -2823,16 +2823,16 @@
         <v>121</v>
       </c>
       <c r="B118" t="n">
-        <v>135</v>
+        <v>110</v>
       </c>
       <c r="C118" t="n">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="D118" t="n">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E118" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="119">
@@ -2840,16 +2840,16 @@
         <v>122</v>
       </c>
       <c r="B119" t="n">
-        <v>110</v>
+        <v>137</v>
       </c>
       <c r="C119" t="n">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D119" t="n">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E119" t="n">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="120">
@@ -2857,16 +2857,16 @@
         <v>123</v>
       </c>
       <c r="B120" t="n">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C120" t="n">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D120" t="n">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E120" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="121">
@@ -2874,16 +2874,16 @@
         <v>124</v>
       </c>
       <c r="B121" t="n">
-        <v>137</v>
+        <v>110</v>
       </c>
       <c r="C121" t="n">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="D121" t="n">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E121" t="n">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="122">
@@ -2891,16 +2891,16 @@
         <v>125</v>
       </c>
       <c r="B122" t="n">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="C122" t="n">
         <v>3</v>
       </c>
       <c r="D122" t="n">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="E122" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="123">
@@ -2908,13 +2908,13 @@
         <v>126</v>
       </c>
       <c r="B123" t="n">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="C123" t="n">
         <v>7</v>
       </c>
       <c r="D123" t="n">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="E123" t="n">
         <v>35</v>
@@ -2925,16 +2925,16 @@
         <v>127</v>
       </c>
       <c r="B124" t="n">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="C124" t="n">
         <v>2</v>
       </c>
       <c r="D124" t="n">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="E124" t="n">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="125">
@@ -2942,13 +2942,13 @@
         <v>128</v>
       </c>
       <c r="B125" t="n">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="C125" t="n">
         <v>2</v>
       </c>
       <c r="D125" t="n">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="E125" t="n">
         <v>36</v>
@@ -2959,16 +2959,16 @@
         <v>129</v>
       </c>
       <c r="B126" t="n">
-        <v>110</v>
+        <v>137</v>
       </c>
       <c r="C126" t="n">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="D126" t="n">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E126" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="127">
@@ -2976,16 +2976,16 @@
         <v>130</v>
       </c>
       <c r="B127" t="n">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="C127" t="n">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="D127" t="n">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E127" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="128">
@@ -2993,16 +2993,16 @@
         <v>131</v>
       </c>
       <c r="B128" t="n">
-        <v>121</v>
+        <v>135</v>
       </c>
       <c r="C128" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D128" t="n">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E128" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="129">
@@ -3013,10 +3013,10 @@
         <v>110</v>
       </c>
       <c r="C129" t="n">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D129" t="n">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E129" t="n">
         <v>30</v>
@@ -3027,16 +3027,16 @@
         <v>133</v>
       </c>
       <c r="B130" t="n">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C130" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D130" t="n">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E130" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="131">
@@ -3044,16 +3044,16 @@
         <v>134</v>
       </c>
       <c r="B131" t="n">
-        <v>110</v>
+        <v>139</v>
       </c>
       <c r="C131" t="n">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="D131" t="n">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E131" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="132">
@@ -3064,13 +3064,13 @@
         <v>110</v>
       </c>
       <c r="C132" t="n">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D132" t="n">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E132" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="133">
@@ -3081,13 +3081,13 @@
         <v>110</v>
       </c>
       <c r="C133" t="n">
+        <v>30</v>
+      </c>
+      <c r="D133" t="n">
+        <v>30</v>
+      </c>
+      <c r="E133" t="n">
         <v>24</v>
-      </c>
-      <c r="D133" t="n">
-        <v>24</v>
-      </c>
-      <c r="E133" t="n">
-        <v>27</v>
       </c>
     </row>
     <row r="134">
@@ -3095,16 +3095,16 @@
         <v>137</v>
       </c>
       <c r="B134" t="n">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="C134" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D134" t="n">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E134" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="135">
@@ -3112,16 +3112,16 @@
         <v>138</v>
       </c>
       <c r="B135" t="n">
-        <v>110</v>
+        <v>135</v>
       </c>
       <c r="C135" t="n">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="D135" t="n">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E135" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="136">
@@ -3129,16 +3129,16 @@
         <v>139</v>
       </c>
       <c r="B136" t="n">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="C136" t="n">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="D136" t="n">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E136" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="137">
@@ -3146,13 +3146,13 @@
         <v>140</v>
       </c>
       <c r="B137" t="n">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C137" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D137" t="n">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E137" t="n">
         <v>22</v>
@@ -3163,16 +3163,16 @@
         <v>141</v>
       </c>
       <c r="B138" t="n">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C138" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D138" t="n">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E138" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="139">
@@ -3180,16 +3180,16 @@
         <v>142</v>
       </c>
       <c r="B139" t="n">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="C139" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D139" t="n">
+        <v>28</v>
+      </c>
+      <c r="E139" t="n">
         <v>21</v>
-      </c>
-      <c r="E139" t="n">
-        <v>18</v>
       </c>
     </row>
     <row r="140">
@@ -3197,16 +3197,16 @@
         <v>143</v>
       </c>
       <c r="B140" t="n">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C140" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D140" t="n">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E140" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="141">
@@ -3214,16 +3214,16 @@
         <v>144</v>
       </c>
       <c r="B141" t="n">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="C141" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D141" t="n">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E141" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="142">
@@ -3231,16 +3231,16 @@
         <v>145</v>
       </c>
       <c r="B142" t="n">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="C142" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D142" t="n">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E142" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="143">
@@ -3248,16 +3248,16 @@
         <v>146</v>
       </c>
       <c r="B143" t="n">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="C143" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D143" t="n">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E143" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="144">
@@ -3265,16 +3265,16 @@
         <v>147</v>
       </c>
       <c r="B144" t="n">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="C144" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D144" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E144" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="145">
@@ -3282,13 +3282,13 @@
         <v>148</v>
       </c>
       <c r="B145" t="n">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C145" t="n">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="D145" t="n">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="E145" t="n">
         <v>14</v>
@@ -3299,16 +3299,16 @@
         <v>149</v>
       </c>
       <c r="B146" t="n">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="C146" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D146" t="n">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E146" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="147">
@@ -3319,13 +3319,13 @@
         <v>110</v>
       </c>
       <c r="C147" t="n">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D147" t="n">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E147" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="148">
@@ -3333,13 +3333,13 @@
         <v>151</v>
       </c>
       <c r="B148" t="n">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="C148" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D148" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E148" t="n">
         <v>11</v>
@@ -3350,16 +3350,16 @@
         <v>152</v>
       </c>
       <c r="B149" t="n">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="C149" t="n">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="D149" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E149" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="150">
@@ -3370,13 +3370,13 @@
         <v>110</v>
       </c>
       <c r="C150" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D150" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E150" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="151">
@@ -3387,10 +3387,10 @@
         <v>110</v>
       </c>
       <c r="C151" t="n">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D151" t="n">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E151" t="n">
         <v>8</v>
@@ -3401,13 +3401,13 @@
         <v>155</v>
       </c>
       <c r="B152" t="n">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="C152" t="n">
         <v>1</v>
       </c>
       <c r="D152" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E152" t="n">
         <v>7</v>
@@ -3438,10 +3438,10 @@
         <v>110</v>
       </c>
       <c r="C154" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D154" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E154" t="n">
         <v>5</v>
@@ -3452,16 +3452,16 @@
         <v>158</v>
       </c>
       <c r="B155" t="n">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C155" t="n">
         <v>5</v>
       </c>
       <c r="D155" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E155" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="156">
@@ -3469,16 +3469,16 @@
         <v>159</v>
       </c>
       <c r="B156" t="n">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C156" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D156" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E156" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="157">
@@ -3489,13 +3489,13 @@
         <v>110</v>
       </c>
       <c r="C157" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D157" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E157" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="158">
@@ -3512,7 +3512,7 @@
         <v>0</v>
       </c>
       <c r="E158" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
calculate missing and non-zero stats
</commit_message>
<xml_diff>
--- a/stats_country_ranks.xlsx
+++ b/stats_country_ranks.xlsx
@@ -1353,7 +1353,7 @@
         <v>123</v>
       </c>
       <c r="E31" t="n">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="32">
@@ -1370,7 +1370,7 @@
         <v>123</v>
       </c>
       <c r="E32" t="n">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33">
@@ -1574,7 +1574,7 @@
         <v>104</v>
       </c>
       <c r="E44" t="n">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="45">
@@ -1591,7 +1591,7 @@
         <v>104</v>
       </c>
       <c r="E45" t="n">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="46">
@@ -1642,7 +1642,7 @@
         <v>96</v>
       </c>
       <c r="E48" t="n">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49">
@@ -1659,7 +1659,7 @@
         <v>96</v>
       </c>
       <c r="E49" t="n">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="50">
@@ -1693,7 +1693,7 @@
         <v>90</v>
       </c>
       <c r="E51" t="n">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="52">
@@ -1710,7 +1710,7 @@
         <v>90</v>
       </c>
       <c r="E52" t="n">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="53">
@@ -1727,7 +1727,7 @@
         <v>83</v>
       </c>
       <c r="E53" t="n">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="54">
@@ -1744,7 +1744,7 @@
         <v>83</v>
       </c>
       <c r="E54" t="n">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="55">
@@ -1999,7 +1999,7 @@
         <v>62</v>
       </c>
       <c r="E69" t="n">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="70">
@@ -2016,7 +2016,7 @@
         <v>62</v>
       </c>
       <c r="E70" t="n">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="71">
@@ -2118,7 +2118,7 @@
         <v>52</v>
       </c>
       <c r="E76" t="n">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="77">
@@ -2135,7 +2135,7 @@
         <v>52</v>
       </c>
       <c r="E77" t="n">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="78">
@@ -2152,7 +2152,7 @@
         <v>52</v>
       </c>
       <c r="E78" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="79">
@@ -2169,7 +2169,7 @@
         <v>52</v>
       </c>
       <c r="E79" t="n">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="80">
@@ -2186,7 +2186,7 @@
         <v>51</v>
       </c>
       <c r="E80" t="n">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="81">
@@ -2203,7 +2203,7 @@
         <v>51</v>
       </c>
       <c r="E81" t="n">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="82">
@@ -2220,7 +2220,7 @@
         <v>50</v>
       </c>
       <c r="E82" t="n">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="83">
@@ -2237,7 +2237,7 @@
         <v>50</v>
       </c>
       <c r="E83" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="84">
@@ -2288,7 +2288,7 @@
         <v>49</v>
       </c>
       <c r="E86" t="n">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="87">
@@ -2305,7 +2305,7 @@
         <v>49</v>
       </c>
       <c r="E87" t="n">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="88">
@@ -2322,7 +2322,7 @@
         <v>49</v>
       </c>
       <c r="E88" t="n">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="89">
@@ -2339,7 +2339,7 @@
         <v>47</v>
       </c>
       <c r="E89" t="n">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="90">
@@ -2390,7 +2390,7 @@
         <v>47</v>
       </c>
       <c r="E92" t="n">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="93">
@@ -2475,7 +2475,7 @@
         <v>43</v>
       </c>
       <c r="E97" t="n">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="98">
@@ -2492,7 +2492,7 @@
         <v>43</v>
       </c>
       <c r="E98" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="99">
@@ -2526,7 +2526,7 @@
         <v>43</v>
       </c>
       <c r="E100" t="n">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="101">
@@ -2543,7 +2543,7 @@
         <v>42</v>
       </c>
       <c r="E101" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="102">
@@ -2560,7 +2560,7 @@
         <v>42</v>
       </c>
       <c r="E102" t="n">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="103">
@@ -2594,7 +2594,7 @@
         <v>41</v>
       </c>
       <c r="E104" t="n">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="105">
@@ -2611,7 +2611,7 @@
         <v>41</v>
       </c>
       <c r="E105" t="n">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="106">
@@ -2696,7 +2696,7 @@
         <v>36</v>
       </c>
       <c r="E110" t="n">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="111">
@@ -2713,7 +2713,7 @@
         <v>36</v>
       </c>
       <c r="E111" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="112">
@@ -2730,7 +2730,7 @@
         <v>36</v>
       </c>
       <c r="E112" t="n">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="113">
@@ -2747,7 +2747,7 @@
         <v>36</v>
       </c>
       <c r="E113" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="114">
@@ -2764,7 +2764,7 @@
         <v>36</v>
       </c>
       <c r="E114" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="115">
@@ -2815,7 +2815,7 @@
         <v>34</v>
       </c>
       <c r="E117" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="118">
@@ -2832,7 +2832,7 @@
         <v>34</v>
       </c>
       <c r="E118" t="n">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="119">
@@ -2849,7 +2849,7 @@
         <v>34</v>
       </c>
       <c r="E119" t="n">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="120">
@@ -2866,7 +2866,7 @@
         <v>34</v>
       </c>
       <c r="E120" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="121">
@@ -2883,7 +2883,7 @@
         <v>34</v>
       </c>
       <c r="E121" t="n">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="122">
@@ -2900,7 +2900,7 @@
         <v>33</v>
       </c>
       <c r="E122" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="123">
@@ -2917,7 +2917,7 @@
         <v>33</v>
       </c>
       <c r="E123" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="124">
@@ -2934,7 +2934,7 @@
         <v>33</v>
       </c>
       <c r="E124" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="125">
@@ -2951,7 +2951,7 @@
         <v>33</v>
       </c>
       <c r="E125" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="126">
@@ -2985,7 +2985,7 @@
         <v>32</v>
       </c>
       <c r="E127" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="128">
@@ -3002,7 +3002,7 @@
         <v>32</v>
       </c>
       <c r="E128" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="129">
@@ -3019,7 +3019,7 @@
         <v>31</v>
       </c>
       <c r="E129" t="n">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="130">
@@ -3053,7 +3053,7 @@
         <v>31</v>
       </c>
       <c r="E131" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="132">
@@ -3087,7 +3087,7 @@
         <v>30</v>
       </c>
       <c r="E133" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="134">
@@ -3104,7 +3104,7 @@
         <v>30</v>
       </c>
       <c r="E134" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="135">
@@ -3121,7 +3121,7 @@
         <v>30</v>
       </c>
       <c r="E135" t="n">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="136">
@@ -3138,7 +3138,7 @@
         <v>30</v>
       </c>
       <c r="E136" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="137">
@@ -3172,7 +3172,7 @@
         <v>28</v>
       </c>
       <c r="E138" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="139">
@@ -3189,7 +3189,7 @@
         <v>28</v>
       </c>
       <c r="E139" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="140">
@@ -3206,7 +3206,7 @@
         <v>27</v>
       </c>
       <c r="E140" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="141">
@@ -3240,7 +3240,7 @@
         <v>27</v>
       </c>
       <c r="E142" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="143">
@@ -3257,7 +3257,7 @@
         <v>27</v>
       </c>
       <c r="E143" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="144">
@@ -3342,7 +3342,7 @@
         <v>23</v>
       </c>
       <c r="E148" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="149">
@@ -3359,7 +3359,7 @@
         <v>23</v>
       </c>
       <c r="E149" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="150">
@@ -3376,7 +3376,7 @@
         <v>21</v>
       </c>
       <c r="E150" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="151">
@@ -3393,7 +3393,7 @@
         <v>21</v>
       </c>
       <c r="E151" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="152">
@@ -3461,7 +3461,7 @@
         <v>6</v>
       </c>
       <c r="E155" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="156">
@@ -3478,7 +3478,7 @@
         <v>6</v>
       </c>
       <c r="E156" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="157">

</xml_diff>

<commit_message>
calculate missing and non-zero stats v2
</commit_message>
<xml_diff>
--- a/stats_country_ranks.xlsx
+++ b/stats_country_ranks.xlsx
@@ -1098,7 +1098,7 @@
         <v>204</v>
       </c>
       <c r="E16" t="n">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17">
@@ -1115,7 +1115,7 @@
         <v>204</v>
       </c>
       <c r="E17" t="n">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18">
@@ -1353,7 +1353,7 @@
         <v>123</v>
       </c>
       <c r="E31" t="n">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32">
@@ -1370,7 +1370,7 @@
         <v>123</v>
       </c>
       <c r="E32" t="n">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33">
@@ -1727,7 +1727,7 @@
         <v>83</v>
       </c>
       <c r="E53" t="n">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="54">
@@ -1744,7 +1744,7 @@
         <v>83</v>
       </c>
       <c r="E54" t="n">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="55">
@@ -1829,7 +1829,7 @@
         <v>76</v>
       </c>
       <c r="E59" t="n">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="60">
@@ -1846,7 +1846,7 @@
         <v>76</v>
       </c>
       <c r="E60" t="n">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="61">
@@ -1897,7 +1897,7 @@
         <v>73</v>
       </c>
       <c r="E63" t="n">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="64">
@@ -1914,7 +1914,7 @@
         <v>73</v>
       </c>
       <c r="E64" t="n">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="65">
@@ -1999,7 +1999,7 @@
         <v>62</v>
       </c>
       <c r="E69" t="n">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="70">
@@ -2016,7 +2016,7 @@
         <v>62</v>
       </c>
       <c r="E70" t="n">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="71">
@@ -2118,7 +2118,7 @@
         <v>52</v>
       </c>
       <c r="E76" t="n">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="77">
@@ -2135,7 +2135,7 @@
         <v>52</v>
       </c>
       <c r="E77" t="n">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="78">
@@ -2152,7 +2152,7 @@
         <v>52</v>
       </c>
       <c r="E78" t="n">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="79">
@@ -2186,7 +2186,7 @@
         <v>51</v>
       </c>
       <c r="E80" t="n">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="81">
@@ -2203,7 +2203,7 @@
         <v>51</v>
       </c>
       <c r="E81" t="n">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="82">
@@ -2220,7 +2220,7 @@
         <v>50</v>
       </c>
       <c r="E82" t="n">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="83">
@@ -2237,7 +2237,7 @@
         <v>50</v>
       </c>
       <c r="E83" t="n">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="84">
@@ -2254,7 +2254,7 @@
         <v>50</v>
       </c>
       <c r="E84" t="n">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="85">
@@ -2288,7 +2288,7 @@
         <v>49</v>
       </c>
       <c r="E86" t="n">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="87">
@@ -2305,7 +2305,7 @@
         <v>49</v>
       </c>
       <c r="E87" t="n">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="88">
@@ -2322,7 +2322,7 @@
         <v>49</v>
       </c>
       <c r="E88" t="n">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="89">
@@ -2339,7 +2339,7 @@
         <v>47</v>
       </c>
       <c r="E89" t="n">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="90">
@@ -2356,7 +2356,7 @@
         <v>47</v>
       </c>
       <c r="E90" t="n">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="91">
@@ -2373,7 +2373,7 @@
         <v>47</v>
       </c>
       <c r="E91" t="n">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="92">
@@ -2441,7 +2441,7 @@
         <v>45</v>
       </c>
       <c r="E95" t="n">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="96">
@@ -2458,7 +2458,7 @@
         <v>45</v>
       </c>
       <c r="E96" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="97">
@@ -2475,7 +2475,7 @@
         <v>43</v>
       </c>
       <c r="E97" t="n">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="98">
@@ -2492,7 +2492,7 @@
         <v>43</v>
       </c>
       <c r="E98" t="n">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="99">
@@ -2509,7 +2509,7 @@
         <v>43</v>
       </c>
       <c r="E99" t="n">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="100">
@@ -2526,7 +2526,7 @@
         <v>43</v>
       </c>
       <c r="E100" t="n">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="101">
@@ -2543,7 +2543,7 @@
         <v>42</v>
       </c>
       <c r="E101" t="n">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="102">
@@ -2560,7 +2560,7 @@
         <v>42</v>
       </c>
       <c r="E102" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="103">
@@ -2577,7 +2577,7 @@
         <v>41</v>
       </c>
       <c r="E103" t="n">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="104">
@@ -2611,7 +2611,7 @@
         <v>41</v>
       </c>
       <c r="E105" t="n">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="106">
@@ -2696,7 +2696,7 @@
         <v>36</v>
       </c>
       <c r="E110" t="n">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="111">
@@ -2713,7 +2713,7 @@
         <v>36</v>
       </c>
       <c r="E111" t="n">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="112">
@@ -2730,7 +2730,7 @@
         <v>36</v>
       </c>
       <c r="E112" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="113">
@@ -2747,7 +2747,7 @@
         <v>36</v>
       </c>
       <c r="E113" t="n">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="114">
@@ -2764,7 +2764,7 @@
         <v>36</v>
       </c>
       <c r="E114" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="115">
@@ -2781,7 +2781,7 @@
         <v>35</v>
       </c>
       <c r="E115" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="116">
@@ -2798,7 +2798,7 @@
         <v>35</v>
       </c>
       <c r="E116" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="117">
@@ -2815,7 +2815,7 @@
         <v>34</v>
       </c>
       <c r="E117" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="118">
@@ -2832,7 +2832,7 @@
         <v>34</v>
       </c>
       <c r="E118" t="n">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="119">
@@ -2849,7 +2849,7 @@
         <v>34</v>
       </c>
       <c r="E119" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="120">
@@ -2866,7 +2866,7 @@
         <v>34</v>
       </c>
       <c r="E120" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="121">
@@ -2883,7 +2883,7 @@
         <v>34</v>
       </c>
       <c r="E121" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="122">
@@ -2900,7 +2900,7 @@
         <v>33</v>
       </c>
       <c r="E122" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="123">
@@ -2917,7 +2917,7 @@
         <v>33</v>
       </c>
       <c r="E123" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="124">
@@ -2934,7 +2934,7 @@
         <v>33</v>
       </c>
       <c r="E124" t="n">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="125">
@@ -2951,7 +2951,7 @@
         <v>33</v>
       </c>
       <c r="E125" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="126">
@@ -2968,7 +2968,7 @@
         <v>32</v>
       </c>
       <c r="E126" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="127">
@@ -2985,7 +2985,7 @@
         <v>32</v>
       </c>
       <c r="E127" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="128">
@@ -3002,7 +3002,7 @@
         <v>32</v>
       </c>
       <c r="E128" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="129">
@@ -3019,7 +3019,7 @@
         <v>31</v>
       </c>
       <c r="E129" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="130">
@@ -3036,7 +3036,7 @@
         <v>31</v>
       </c>
       <c r="E130" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="131">
@@ -3053,7 +3053,7 @@
         <v>31</v>
       </c>
       <c r="E131" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="132">
@@ -3070,7 +3070,7 @@
         <v>31</v>
       </c>
       <c r="E132" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="133">
@@ -3087,7 +3087,7 @@
         <v>30</v>
       </c>
       <c r="E133" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="134">
@@ -3104,7 +3104,7 @@
         <v>30</v>
       </c>
       <c r="E134" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="135">
@@ -3138,7 +3138,7 @@
         <v>30</v>
       </c>
       <c r="E136" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="137">
@@ -3206,7 +3206,7 @@
         <v>27</v>
       </c>
       <c r="E140" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="141">
@@ -3223,7 +3223,7 @@
         <v>27</v>
       </c>
       <c r="E141" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="142">
@@ -3240,7 +3240,7 @@
         <v>27</v>
       </c>
       <c r="E142" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="143">
@@ -3257,7 +3257,7 @@
         <v>27</v>
       </c>
       <c r="E143" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="144">
@@ -3342,7 +3342,7 @@
         <v>23</v>
       </c>
       <c r="E148" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="149">
@@ -3359,7 +3359,7 @@
         <v>23</v>
       </c>
       <c r="E149" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="150">

</xml_diff>

<commit_message>
calculate missing stats again
</commit_message>
<xml_diff>
--- a/stats_country_ranks.xlsx
+++ b/stats_country_ranks.xlsx
@@ -1098,7 +1098,7 @@
         <v>204</v>
       </c>
       <c r="E16" t="n">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17">
@@ -1115,7 +1115,7 @@
         <v>204</v>
       </c>
       <c r="E17" t="n">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18">
@@ -1353,7 +1353,7 @@
         <v>123</v>
       </c>
       <c r="E31" t="n">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="32">
@@ -1370,7 +1370,7 @@
         <v>123</v>
       </c>
       <c r="E32" t="n">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33">
@@ -1999,7 +1999,7 @@
         <v>62</v>
       </c>
       <c r="E69" t="n">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="70">
@@ -2016,7 +2016,7 @@
         <v>62</v>
       </c>
       <c r="E70" t="n">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="71">
@@ -2118,7 +2118,7 @@
         <v>52</v>
       </c>
       <c r="E76" t="n">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="77">
@@ -2135,7 +2135,7 @@
         <v>52</v>
       </c>
       <c r="E77" t="n">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="78">
@@ -2152,7 +2152,7 @@
         <v>52</v>
       </c>
       <c r="E78" t="n">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="79">
@@ -2169,7 +2169,7 @@
         <v>52</v>
       </c>
       <c r="E79" t="n">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="80">
@@ -2220,7 +2220,7 @@
         <v>50</v>
       </c>
       <c r="E82" t="n">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="83">
@@ -2254,7 +2254,7 @@
         <v>50</v>
       </c>
       <c r="E84" t="n">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="85">
@@ -2288,7 +2288,7 @@
         <v>49</v>
       </c>
       <c r="E86" t="n">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="87">
@@ -2305,7 +2305,7 @@
         <v>49</v>
       </c>
       <c r="E87" t="n">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="88">
@@ -2339,7 +2339,7 @@
         <v>47</v>
       </c>
       <c r="E89" t="n">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="90">
@@ -2356,7 +2356,7 @@
         <v>47</v>
       </c>
       <c r="E90" t="n">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="91">
@@ -2390,7 +2390,7 @@
         <v>47</v>
       </c>
       <c r="E92" t="n">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="93">
@@ -2407,7 +2407,7 @@
         <v>46</v>
       </c>
       <c r="E93" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="94">
@@ -2424,7 +2424,7 @@
         <v>46</v>
       </c>
       <c r="E94" t="n">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="95">
@@ -2441,7 +2441,7 @@
         <v>45</v>
       </c>
       <c r="E95" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="96">
@@ -2458,7 +2458,7 @@
         <v>45</v>
       </c>
       <c r="E96" t="n">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="97">
@@ -2492,7 +2492,7 @@
         <v>43</v>
       </c>
       <c r="E98" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="99">
@@ -2509,7 +2509,7 @@
         <v>43</v>
       </c>
       <c r="E99" t="n">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="100">
@@ -2526,7 +2526,7 @@
         <v>43</v>
       </c>
       <c r="E100" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="101">
@@ -2577,7 +2577,7 @@
         <v>41</v>
       </c>
       <c r="E103" t="n">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="104">
@@ -2611,7 +2611,7 @@
         <v>41</v>
       </c>
       <c r="E105" t="n">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="106">
@@ -2645,7 +2645,7 @@
         <v>39</v>
       </c>
       <c r="E107" t="n">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="108">
@@ -2662,7 +2662,7 @@
         <v>39</v>
       </c>
       <c r="E108" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="109">
@@ -2696,7 +2696,7 @@
         <v>36</v>
       </c>
       <c r="E110" t="n">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="111">
@@ -2713,7 +2713,7 @@
         <v>36</v>
       </c>
       <c r="E111" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="112">
@@ -2747,7 +2747,7 @@
         <v>36</v>
       </c>
       <c r="E113" t="n">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="114">
@@ -2764,7 +2764,7 @@
         <v>36</v>
       </c>
       <c r="E114" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="115">
@@ -2832,7 +2832,7 @@
         <v>34</v>
       </c>
       <c r="E118" t="n">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="119">
@@ -2849,7 +2849,7 @@
         <v>34</v>
       </c>
       <c r="E119" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="120">
@@ -2866,7 +2866,7 @@
         <v>34</v>
       </c>
       <c r="E120" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="121">
@@ -2883,7 +2883,7 @@
         <v>34</v>
       </c>
       <c r="E121" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="122">
@@ -2900,7 +2900,7 @@
         <v>33</v>
       </c>
       <c r="E122" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="123">
@@ -2917,7 +2917,7 @@
         <v>33</v>
       </c>
       <c r="E123" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="124">
@@ -2968,7 +2968,7 @@
         <v>32</v>
       </c>
       <c r="E126" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="127">
@@ -2985,7 +2985,7 @@
         <v>32</v>
       </c>
       <c r="E127" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="128">
@@ -3002,7 +3002,7 @@
         <v>32</v>
       </c>
       <c r="E128" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="129">
@@ -3019,7 +3019,7 @@
         <v>31</v>
       </c>
       <c r="E129" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="130">
@@ -3036,7 +3036,7 @@
         <v>31</v>
       </c>
       <c r="E130" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="131">
@@ -3053,7 +3053,7 @@
         <v>31</v>
       </c>
       <c r="E131" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="132">
@@ -3087,7 +3087,7 @@
         <v>30</v>
       </c>
       <c r="E133" t="n">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="134">
@@ -3104,7 +3104,7 @@
         <v>30</v>
       </c>
       <c r="E134" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="135">
@@ -3121,7 +3121,7 @@
         <v>30</v>
       </c>
       <c r="E135" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="136">
@@ -3138,7 +3138,7 @@
         <v>30</v>
       </c>
       <c r="E136" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="137">
@@ -3206,7 +3206,7 @@
         <v>27</v>
       </c>
       <c r="E140" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="141">
@@ -3223,7 +3223,7 @@
         <v>27</v>
       </c>
       <c r="E141" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="142">
@@ -3240,7 +3240,7 @@
         <v>27</v>
       </c>
       <c r="E142" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="143">
@@ -3257,7 +3257,7 @@
         <v>27</v>
       </c>
       <c r="E143" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="144">
@@ -3342,7 +3342,7 @@
         <v>23</v>
       </c>
       <c r="E148" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="149">
@@ -3359,7 +3359,7 @@
         <v>23</v>
       </c>
       <c r="E149" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="150">
@@ -3427,7 +3427,7 @@
         <v>9</v>
       </c>
       <c r="E153" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="154">
@@ -3444,7 +3444,7 @@
         <v>9</v>
       </c>
       <c r="E154" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="155">
@@ -3461,7 +3461,7 @@
         <v>6</v>
       </c>
       <c r="E155" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="156">
@@ -3478,7 +3478,7 @@
         <v>6</v>
       </c>
       <c r="E156" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="157">

</xml_diff>